<commit_message>
added val_loss, pytorch optimizations
</commit_message>
<xml_diff>
--- a/data/fptp_labeled.xlsx
+++ b/data/fptp_labeled.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliotsilva/Desktop/DS-GA-1006/FairFrame/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56C08770-3ED9-7A42-A4EA-145D6E5CB014}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B3C93BA-0C13-BF4C-A0F2-2C662CB266D8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="680" yWindow="460" windowWidth="28800" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="235" uniqueCount="166">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="165">
   <si>
     <t>review</t>
   </si>
@@ -29,9 +29,6 @@
   </si>
   <si>
     <t>flagged_index</t>
-  </si>
-  <si>
-    <t>problematic</t>
   </si>
   <si>
     <t>['flexible', ',', 'creative', 'and', 'made', 'my', 'vision', 'a', 'reality', '.']</t>
@@ -576,12 +573,16 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
       <right style="thin">
         <color auto="1"/>
       </right>
       <top/>
-      <bottom/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -898,19 +899,19 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F501"/>
+  <dimension ref="A1:E501"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" zoomScale="200" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="D118" sqref="D118"/>
+    <sheetView tabSelected="1" zoomScale="134" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="101.6640625" customWidth="1"/>
+    <col min="2" max="2" width="95.5" customWidth="1"/>
     <col min="3" max="3" width="13.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -920,22 +921,19 @@
       <c r="D1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>165</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E1" s="2" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="1">
         <v>121269</v>
       </c>
       <c r="B2" t="s">
+        <v>3</v>
+      </c>
+      <c r="C2" t="s">
         <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
       </c>
       <c r="D2">
         <v>2</v>
@@ -943,39 +941,33 @@
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
         <v>134304</v>
       </c>
       <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="s">
         <v>6</v>
-      </c>
-      <c r="C3" t="s">
-        <v>7</v>
       </c>
       <c r="D3">
         <v>5</v>
       </c>
       <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
         <v>40630</v>
       </c>
       <c r="B4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C4" t="s">
         <v>8</v>
-      </c>
-      <c r="C4" t="s">
-        <v>9</v>
       </c>
       <c r="D4">
         <v>8</v>
@@ -983,59 +975,50 @@
       <c r="E4">
         <v>1</v>
       </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
         <v>33052</v>
       </c>
       <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
         <v>10</v>
-      </c>
-      <c r="C5" t="s">
-        <v>11</v>
       </c>
       <c r="D5">
         <v>7</v>
       </c>
       <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
         <v>-1</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>71109</v>
       </c>
       <c r="B6" t="s">
+        <v>11</v>
+      </c>
+      <c r="C6" t="s">
         <v>12</v>
-      </c>
-      <c r="C6" t="s">
-        <v>13</v>
       </c>
       <c r="D6">
         <v>6</v>
       </c>
       <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>67918</v>
       </c>
       <c r="B7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C7" t="s">
         <v>14</v>
-      </c>
-      <c r="C7" t="s">
-        <v>15</v>
       </c>
       <c r="D7">
         <v>10</v>
@@ -1043,19 +1026,16 @@
       <c r="E7">
         <v>1</v>
       </c>
-      <c r="F7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>42139</v>
       </c>
       <c r="B8" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" t="s">
         <v>16</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
       </c>
       <c r="D8">
         <v>3</v>
@@ -1063,159 +1043,135 @@
       <c r="E8">
         <v>1</v>
       </c>
-      <c r="F8">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>22991</v>
       </c>
       <c r="B9" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9">
-        <v>1</v>
-      </c>
-      <c r="F9">
         <v>-1</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>55547</v>
       </c>
       <c r="B10" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" t="s">
         <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>20</v>
       </c>
       <c r="D10">
         <v>5</v>
       </c>
       <c r="E10">
-        <v>1</v>
-      </c>
-      <c r="F10">
         <v>-1</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
         <v>126969</v>
       </c>
       <c r="B11" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" t="s">
         <v>21</v>
       </c>
-      <c r="C11" t="s">
-        <v>22</v>
-      </c>
       <c r="D11">
         <v>1</v>
       </c>
       <c r="E11">
-        <v>1</v>
-      </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
         <v>117682</v>
       </c>
       <c r="B12" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C12" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D12">
         <v>3</v>
       </c>
       <c r="E12">
-        <v>1</v>
-      </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
         <v>121157</v>
       </c>
       <c r="B13" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" t="s">
         <v>24</v>
       </c>
-      <c r="C13" t="s">
-        <v>25</v>
-      </c>
       <c r="D13">
         <v>0</v>
       </c>
       <c r="E13">
-        <v>1</v>
-      </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
         <v>120280</v>
       </c>
       <c r="B14" t="s">
+        <v>25</v>
+      </c>
+      <c r="C14" t="s">
         <v>26</v>
-      </c>
-      <c r="C14" t="s">
-        <v>27</v>
       </c>
       <c r="D14">
         <v>18</v>
       </c>
       <c r="E14">
-        <v>1</v>
-      </c>
-      <c r="F14">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
         <v>65500</v>
       </c>
       <c r="B15" t="s">
+        <v>27</v>
+      </c>
+      <c r="C15" t="s">
         <v>28</v>
-      </c>
-      <c r="C15" t="s">
-        <v>29</v>
       </c>
       <c r="D15">
         <v>5</v>
       </c>
       <c r="E15">
-        <v>1</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
         <v>96602</v>
       </c>
       <c r="B16" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" t="s">
         <v>30</v>
-      </c>
-      <c r="C16" t="s">
-        <v>31</v>
       </c>
       <c r="D16">
         <v>2</v>
@@ -1223,39 +1179,33 @@
       <c r="E16">
         <v>1</v>
       </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
         <v>58588</v>
       </c>
       <c r="B17" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" t="s">
         <v>32</v>
       </c>
-      <c r="C17" t="s">
-        <v>33</v>
-      </c>
       <c r="D17">
         <v>1</v>
       </c>
       <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
         <v>47152</v>
       </c>
       <c r="B18" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C18" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D18">
         <v>3</v>
@@ -1263,19 +1213,16 @@
       <c r="E18">
         <v>1</v>
       </c>
-      <c r="F18">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
         <v>117850</v>
       </c>
       <c r="B19" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C19" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D19">
         <v>2</v>
@@ -1283,39 +1230,33 @@
       <c r="E19">
         <v>1</v>
       </c>
-      <c r="F19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
         <v>82900</v>
       </c>
       <c r="B20" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" t="s">
         <v>36</v>
-      </c>
-      <c r="C20" t="s">
-        <v>37</v>
       </c>
       <c r="D20">
         <v>11</v>
       </c>
       <c r="E20">
-        <v>1</v>
-      </c>
-      <c r="F20">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
         <v>14637</v>
       </c>
       <c r="B21" t="s">
+        <v>37</v>
+      </c>
+      <c r="C21" t="s">
         <v>38</v>
-      </c>
-      <c r="C21" t="s">
-        <v>39</v>
       </c>
       <c r="D21">
         <v>2</v>
@@ -1323,19 +1264,16 @@
       <c r="E21">
         <v>1</v>
       </c>
-      <c r="F21">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
         <v>135248</v>
       </c>
       <c r="B22" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C22" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D22">
         <v>1</v>
@@ -1343,79 +1281,67 @@
       <c r="E22">
         <v>1</v>
       </c>
-      <c r="F22">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
         <v>105413</v>
       </c>
       <c r="B23" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" t="s">
         <v>41</v>
-      </c>
-      <c r="C23" t="s">
-        <v>42</v>
       </c>
       <c r="D23">
         <v>17</v>
       </c>
       <c r="E23">
-        <v>1</v>
-      </c>
-      <c r="F23">
         <v>-1</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
         <v>9133</v>
       </c>
       <c r="B24" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C24" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D24">
         <v>0</v>
       </c>
       <c r="E24">
-        <v>1</v>
-      </c>
-      <c r="F24">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
         <v>88520</v>
       </c>
       <c r="B25" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C25" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D25">
         <v>4</v>
       </c>
       <c r="E25">
-        <v>1</v>
-      </c>
-      <c r="F25">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
         <v>86653</v>
       </c>
       <c r="B26" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C26" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D26">
         <v>2</v>
@@ -1423,19 +1349,16 @@
       <c r="E26">
         <v>1</v>
       </c>
-      <c r="F26">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
         <v>57640</v>
       </c>
       <c r="B27" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C27" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D27">
         <v>6</v>
@@ -1443,59 +1366,50 @@
       <c r="E27">
         <v>1</v>
       </c>
-      <c r="F27">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
         <v>62929</v>
       </c>
       <c r="B28" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C28" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D28">
         <v>3</v>
       </c>
       <c r="E28">
-        <v>1</v>
-      </c>
-      <c r="F28">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
         <v>81451</v>
       </c>
       <c r="B29" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C29" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D29">
         <v>0</v>
       </c>
       <c r="E29">
-        <v>1</v>
-      </c>
-      <c r="F29">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
         <v>16159</v>
       </c>
       <c r="B30" t="s">
+        <v>48</v>
+      </c>
+      <c r="C30" t="s">
         <v>49</v>
-      </c>
-      <c r="C30" t="s">
-        <v>50</v>
       </c>
       <c r="D30">
         <v>2</v>
@@ -1503,19 +1417,16 @@
       <c r="E30">
         <v>1</v>
       </c>
-      <c r="F30">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
         <v>130362</v>
       </c>
       <c r="B31" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="C31" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D31">
         <v>6</v>
@@ -1523,79 +1434,67 @@
       <c r="E31">
         <v>1</v>
       </c>
-      <c r="F31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
         <v>30657</v>
       </c>
       <c r="B32" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C32" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D32">
         <v>11</v>
       </c>
       <c r="E32">
-        <v>1</v>
-      </c>
-      <c r="F32">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
         <v>15243</v>
       </c>
       <c r="B33" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="C33" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D33">
         <v>0</v>
       </c>
       <c r="E33">
-        <v>1</v>
-      </c>
-      <c r="F33">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
         <v>71474</v>
       </c>
       <c r="B34" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C34" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D34">
         <v>0</v>
       </c>
       <c r="E34">
-        <v>1</v>
-      </c>
-      <c r="F34">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>132422</v>
       </c>
       <c r="B35" t="s">
+        <v>54</v>
+      </c>
+      <c r="C35" t="s">
         <v>55</v>
-      </c>
-      <c r="C35" t="s">
-        <v>56</v>
       </c>
       <c r="D35">
         <v>3</v>
@@ -1603,79 +1502,67 @@
       <c r="E35">
         <v>1</v>
       </c>
-      <c r="F35">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>28653</v>
       </c>
       <c r="B36" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C36" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D36">
         <v>0</v>
       </c>
       <c r="E36">
-        <v>1</v>
-      </c>
-      <c r="F36">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>129662</v>
       </c>
       <c r="B37" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C37" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D37">
         <v>4</v>
       </c>
       <c r="E37">
-        <v>1</v>
-      </c>
-      <c r="F37">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
         <v>84709</v>
       </c>
       <c r="B38" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C38" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D38">
         <v>0</v>
       </c>
       <c r="E38">
-        <v>1</v>
-      </c>
-      <c r="F38">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
         <v>130122</v>
       </c>
       <c r="B39" t="s">
+        <v>59</v>
+      </c>
+      <c r="C39" t="s">
         <v>60</v>
-      </c>
-      <c r="C39" t="s">
-        <v>61</v>
       </c>
       <c r="D39">
         <v>4</v>
@@ -1683,79 +1570,67 @@
       <c r="E39">
         <v>1</v>
       </c>
-      <c r="F39">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>4059</v>
       </c>
       <c r="B40" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C40" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D40">
         <v>2</v>
       </c>
       <c r="E40">
-        <v>1</v>
-      </c>
-      <c r="F40">
         <v>-1</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>4872</v>
       </c>
       <c r="B41" t="s">
+        <v>62</v>
+      </c>
+      <c r="C41" t="s">
         <v>63</v>
-      </c>
-      <c r="C41" t="s">
-        <v>64</v>
       </c>
       <c r="D41">
         <v>7</v>
       </c>
       <c r="E41">
-        <v>1</v>
-      </c>
-      <c r="F41">
         <v>-1</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
         <v>8887</v>
       </c>
       <c r="B42" t="s">
+        <v>64</v>
+      </c>
+      <c r="C42" t="s">
         <v>65</v>
-      </c>
-      <c r="C42" t="s">
-        <v>66</v>
       </c>
       <c r="D42">
         <v>20</v>
       </c>
       <c r="E42">
-        <v>1</v>
-      </c>
-      <c r="F42">
         <v>-1</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
         <v>46030</v>
       </c>
       <c r="B43" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C43" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D43">
         <v>2</v>
@@ -1763,19 +1638,16 @@
       <c r="E43">
         <v>1</v>
       </c>
-      <c r="F43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
         <v>114112</v>
       </c>
       <c r="B44" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C44" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D44">
         <v>3</v>
@@ -1783,39 +1655,33 @@
       <c r="E44">
         <v>1</v>
       </c>
-      <c r="F44">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>124710</v>
       </c>
       <c r="B45" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="C45" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D45">
         <v>0</v>
       </c>
       <c r="E45">
-        <v>1</v>
-      </c>
-      <c r="F45">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
         <v>61746</v>
       </c>
       <c r="B46" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C46" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D46">
         <v>2</v>
@@ -1823,59 +1689,50 @@
       <c r="E46">
         <v>1</v>
       </c>
-      <c r="F46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
         <v>139029</v>
       </c>
       <c r="B47" t="s">
+        <v>70</v>
+      </c>
+      <c r="C47" t="s">
         <v>71</v>
       </c>
-      <c r="C47" t="s">
-        <v>72</v>
-      </c>
       <c r="D47">
         <v>1</v>
       </c>
       <c r="E47">
         <v>1</v>
       </c>
-      <c r="F47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>129381</v>
       </c>
       <c r="B48" t="s">
+        <v>72</v>
+      </c>
+      <c r="C48" t="s">
         <v>73</v>
-      </c>
-      <c r="C48" t="s">
-        <v>74</v>
       </c>
       <c r="D48">
         <v>2</v>
       </c>
       <c r="E48">
-        <v>1</v>
-      </c>
-      <c r="F48">
         <v>-1</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>32438</v>
       </c>
       <c r="B49" t="s">
+        <v>74</v>
+      </c>
+      <c r="C49" t="s">
         <v>75</v>
-      </c>
-      <c r="C49" t="s">
-        <v>76</v>
       </c>
       <c r="D49">
         <v>6</v>
@@ -1883,79 +1740,67 @@
       <c r="E49">
         <v>1</v>
       </c>
-      <c r="F49">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="50" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>102153</v>
       </c>
       <c r="B50" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C50" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D50">
         <v>19</v>
       </c>
       <c r="E50">
-        <v>1</v>
-      </c>
-      <c r="F50">
         <v>-1</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>14881</v>
       </c>
       <c r="B51" t="s">
+        <v>77</v>
+      </c>
+      <c r="C51" t="s">
         <v>78</v>
-      </c>
-      <c r="C51" t="s">
-        <v>79</v>
       </c>
       <c r="D51">
         <v>3</v>
       </c>
       <c r="E51">
-        <v>1</v>
-      </c>
-      <c r="F51">
         <v>-1</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>130610</v>
       </c>
       <c r="B52" t="s">
+        <v>79</v>
+      </c>
+      <c r="C52" t="s">
         <v>80</v>
       </c>
-      <c r="C52" t="s">
-        <v>81</v>
-      </c>
       <c r="D52">
         <v>1</v>
       </c>
       <c r="E52">
         <v>1</v>
       </c>
-      <c r="F52">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="53" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>109345</v>
       </c>
       <c r="B53" t="s">
+        <v>81</v>
+      </c>
+      <c r="C53" t="s">
         <v>82</v>
-      </c>
-      <c r="C53" t="s">
-        <v>83</v>
       </c>
       <c r="D53">
         <v>23</v>
@@ -1963,19 +1808,16 @@
       <c r="E53">
         <v>1</v>
       </c>
-      <c r="F53">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>117179</v>
       </c>
       <c r="B54" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C54" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D54">
         <v>2</v>
@@ -1983,99 +1825,84 @@
       <c r="E54">
         <v>1</v>
       </c>
-      <c r="F54">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="55" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>53661</v>
       </c>
       <c r="B55" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C55" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D55">
         <v>0</v>
       </c>
       <c r="E55">
-        <v>1</v>
-      </c>
-      <c r="F55">
         <v>-1</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>46799</v>
       </c>
       <c r="B56" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="C56" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D56">
         <v>8</v>
       </c>
       <c r="E56">
-        <v>1</v>
-      </c>
-      <c r="F56">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="57" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>75143</v>
       </c>
       <c r="B57" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C57" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D57">
         <v>5</v>
       </c>
       <c r="E57">
-        <v>1</v>
-      </c>
-      <c r="F57">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>61753</v>
       </c>
       <c r="B58" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C58" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D58">
         <v>1</v>
       </c>
       <c r="E58">
-        <v>1</v>
-      </c>
-      <c r="F58">
         <v>-1</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>138055</v>
       </c>
       <c r="B59" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C59" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D59">
         <v>4</v>
@@ -2083,19 +1910,16 @@
       <c r="E59">
         <v>1</v>
       </c>
-      <c r="F59">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="60" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
         <v>75096</v>
       </c>
       <c r="B60" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C60" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D60">
         <v>1</v>
@@ -2103,39 +1927,33 @@
       <c r="E60">
         <v>1</v>
       </c>
-      <c r="F60">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="61" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
         <v>126241</v>
       </c>
       <c r="B61" t="s">
+        <v>90</v>
+      </c>
+      <c r="C61" t="s">
         <v>91</v>
-      </c>
-      <c r="C61" t="s">
-        <v>92</v>
       </c>
       <c r="D61">
         <v>11</v>
       </c>
       <c r="E61">
-        <v>1</v>
-      </c>
-      <c r="F61">
         <v>-1</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>131950</v>
       </c>
       <c r="B62" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C62" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D62">
         <v>5</v>
@@ -2143,39 +1961,33 @@
       <c r="E62">
         <v>1</v>
       </c>
-      <c r="F62">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>128087</v>
       </c>
       <c r="B63" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="C63" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D63">
         <v>0</v>
       </c>
       <c r="E63">
-        <v>1</v>
-      </c>
-      <c r="F63">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>81400</v>
       </c>
       <c r="B64" t="s">
+        <v>94</v>
+      </c>
+      <c r="C64" t="s">
         <v>95</v>
-      </c>
-      <c r="C64" t="s">
-        <v>96</v>
       </c>
       <c r="D64">
         <v>2</v>
@@ -2183,19 +1995,16 @@
       <c r="E64">
         <v>1</v>
       </c>
-      <c r="F64">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="65" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>58311</v>
       </c>
       <c r="B65" t="s">
+        <v>96</v>
+      </c>
+      <c r="C65" t="s">
         <v>97</v>
-      </c>
-      <c r="C65" t="s">
-        <v>98</v>
       </c>
       <c r="D65">
         <v>5</v>
@@ -2203,59 +2012,50 @@
       <c r="E65">
         <v>1</v>
       </c>
-      <c r="F65">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="66" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>71780</v>
       </c>
       <c r="B66" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C66" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D66">
         <v>0</v>
       </c>
       <c r="E66">
-        <v>1</v>
-      </c>
-      <c r="F66">
         <v>-1</v>
       </c>
     </row>
-    <row r="67" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>23434</v>
       </c>
       <c r="B67" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C67" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D67">
         <v>0</v>
       </c>
       <c r="E67">
-        <v>1</v>
-      </c>
-      <c r="F67">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>39540</v>
       </c>
       <c r="B68" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C68" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D68">
         <v>0</v>
@@ -2263,99 +2063,84 @@
       <c r="E68">
         <v>1</v>
       </c>
-      <c r="F68">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="69" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
         <v>49449</v>
       </c>
       <c r="B69" t="s">
+        <v>101</v>
+      </c>
+      <c r="C69" t="s">
         <v>102</v>
-      </c>
-      <c r="C69" t="s">
-        <v>103</v>
       </c>
       <c r="D69">
         <v>5</v>
       </c>
       <c r="E69">
-        <v>1</v>
-      </c>
-      <c r="F69">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>126810</v>
       </c>
       <c r="B70" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C70" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D70">
         <v>3</v>
       </c>
       <c r="E70">
-        <v>1</v>
-      </c>
-      <c r="F70">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
         <v>120200</v>
       </c>
       <c r="B71" t="s">
+        <v>104</v>
+      </c>
+      <c r="C71" t="s">
         <v>105</v>
       </c>
-      <c r="C71" t="s">
-        <v>106</v>
-      </c>
       <c r="D71">
         <v>1</v>
       </c>
       <c r="E71">
         <v>1</v>
       </c>
-      <c r="F71">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="72" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
         <v>117506</v>
       </c>
       <c r="B72" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C72" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D72">
         <v>0</v>
       </c>
       <c r="E72">
-        <v>1</v>
-      </c>
-      <c r="F72">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
         <v>106152</v>
       </c>
       <c r="B73" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C73" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D73">
         <v>3</v>
@@ -2363,19 +2148,16 @@
       <c r="E73">
         <v>1</v>
       </c>
-      <c r="F73">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="74" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>73754</v>
       </c>
       <c r="B74" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="C74" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D74">
         <v>2</v>
@@ -2383,119 +2165,101 @@
       <c r="E74">
         <v>1</v>
       </c>
-      <c r="F74">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="75" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
         <v>61705</v>
       </c>
       <c r="B75" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C75" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D75">
         <v>0</v>
       </c>
       <c r="E75">
-        <v>1</v>
-      </c>
-      <c r="F75">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
         <v>33674</v>
       </c>
       <c r="B76" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="C76" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D76">
         <v>4</v>
       </c>
       <c r="E76">
-        <v>1</v>
-      </c>
-      <c r="F76">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>20429</v>
       </c>
       <c r="B77" t="s">
+        <v>111</v>
+      </c>
+      <c r="C77" t="s">
         <v>112</v>
       </c>
-      <c r="C77" t="s">
-        <v>113</v>
-      </c>
       <c r="D77">
         <v>1</v>
       </c>
       <c r="E77">
         <v>1</v>
       </c>
-      <c r="F77">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="78" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>61268</v>
       </c>
       <c r="B78" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="C78" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D78">
         <v>5</v>
       </c>
       <c r="E78">
-        <v>1</v>
-      </c>
-      <c r="F78">
         <v>-1</v>
       </c>
     </row>
-    <row r="79" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>64994</v>
       </c>
       <c r="B79" t="s">
+        <v>114</v>
+      </c>
+      <c r="C79" t="s">
         <v>115</v>
       </c>
-      <c r="C79" t="s">
-        <v>116</v>
-      </c>
       <c r="D79">
         <v>0</v>
       </c>
       <c r="E79">
-        <v>1</v>
-      </c>
-      <c r="F79">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
         <v>98614</v>
       </c>
       <c r="B80" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C80" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D80">
         <v>0</v>
@@ -2503,19 +2267,16 @@
       <c r="E80">
         <v>1</v>
       </c>
-      <c r="F80">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="81" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>41809</v>
       </c>
       <c r="B81" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C81" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D81">
         <v>9</v>
@@ -2523,19 +2284,16 @@
       <c r="E81">
         <v>1</v>
       </c>
-      <c r="F81">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>17816</v>
       </c>
       <c r="B82" t="s">
+        <v>118</v>
+      </c>
+      <c r="C82" t="s">
         <v>119</v>
-      </c>
-      <c r="C82" t="s">
-        <v>120</v>
       </c>
       <c r="D82">
         <v>2</v>
@@ -2543,59 +2301,50 @@
       <c r="E82">
         <v>1</v>
       </c>
-      <c r="F82">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="83" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
         <v>44551</v>
       </c>
       <c r="B83" t="s">
+        <v>120</v>
+      </c>
+      <c r="C83" t="s">
         <v>121</v>
       </c>
-      <c r="C83" t="s">
-        <v>122</v>
-      </c>
       <c r="D83">
         <v>0</v>
       </c>
       <c r="E83">
         <v>1</v>
       </c>
-      <c r="F83">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>39086</v>
       </c>
       <c r="B84" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C84" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="D84">
         <v>6</v>
       </c>
       <c r="E84">
-        <v>1</v>
-      </c>
-      <c r="F84">
         <v>-1</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
         <v>40657</v>
       </c>
       <c r="B85" t="s">
+        <v>123</v>
+      </c>
+      <c r="C85" t="s">
         <v>124</v>
-      </c>
-      <c r="C85" t="s">
-        <v>125</v>
       </c>
       <c r="D85">
         <v>22</v>
@@ -2603,139 +2352,118 @@
       <c r="E85">
         <v>1</v>
       </c>
-      <c r="F85">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="86" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
         <v>39261</v>
       </c>
       <c r="B86" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="C86" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D86">
         <v>0</v>
       </c>
       <c r="E86">
-        <v>1</v>
-      </c>
-      <c r="F86">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="87" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>45460</v>
       </c>
       <c r="B87" t="s">
+        <v>126</v>
+      </c>
+      <c r="C87" t="s">
         <v>127</v>
       </c>
-      <c r="C87" t="s">
-        <v>128</v>
-      </c>
       <c r="D87">
         <v>1</v>
       </c>
       <c r="E87">
         <v>1</v>
       </c>
-      <c r="F87">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>57054</v>
       </c>
       <c r="B88" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C88" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D88">
         <v>4</v>
       </c>
       <c r="E88">
-        <v>1</v>
-      </c>
-      <c r="F88">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>43363</v>
       </c>
       <c r="B89" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C89" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D89">
         <v>0</v>
       </c>
       <c r="E89">
-        <v>1</v>
-      </c>
-      <c r="F89">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>111518</v>
       </c>
       <c r="B90" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C90" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D90">
         <v>13</v>
       </c>
       <c r="E90">
-        <v>1</v>
-      </c>
-      <c r="F90">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
         <v>27202</v>
       </c>
       <c r="B91" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C91" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D91">
         <v>4</v>
       </c>
       <c r="E91">
-        <v>1</v>
-      </c>
-      <c r="F91">
         <v>-1</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>16589</v>
       </c>
       <c r="B92" t="s">
+        <v>132</v>
+      </c>
+      <c r="C92" t="s">
         <v>133</v>
-      </c>
-      <c r="C92" t="s">
-        <v>134</v>
       </c>
       <c r="D92">
         <v>13</v>
@@ -2743,99 +2471,84 @@
       <c r="E92">
         <v>1</v>
       </c>
-      <c r="F92">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="93" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>92313</v>
       </c>
       <c r="B93" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="C93" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D93">
         <v>0</v>
       </c>
       <c r="E93">
-        <v>1</v>
-      </c>
-      <c r="F93">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>31897</v>
       </c>
       <c r="B94" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="C94" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D94">
         <v>0</v>
       </c>
       <c r="E94">
-        <v>1</v>
-      </c>
-      <c r="F94">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="95" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>32899</v>
       </c>
       <c r="B95" t="s">
+        <v>136</v>
+      </c>
+      <c r="C95" t="s">
         <v>137</v>
-      </c>
-      <c r="C95" t="s">
-        <v>138</v>
       </c>
       <c r="D95">
         <v>2</v>
       </c>
       <c r="E95">
-        <v>1</v>
-      </c>
-      <c r="F95">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="96" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>128070</v>
       </c>
       <c r="B96" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="C96" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D96">
         <v>1</v>
       </c>
       <c r="E96">
-        <v>1</v>
-      </c>
-      <c r="F96">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="97" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>45353</v>
       </c>
       <c r="B97" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="C97" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="D97">
         <v>0</v>
@@ -2843,59 +2556,50 @@
       <c r="E97">
         <v>1</v>
       </c>
-      <c r="F97">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="98" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
         <v>102663</v>
       </c>
       <c r="B98" t="s">
+        <v>140</v>
+      </c>
+      <c r="C98" t="s">
         <v>141</v>
-      </c>
-      <c r="C98" t="s">
-        <v>142</v>
       </c>
       <c r="D98">
         <v>8</v>
       </c>
       <c r="E98">
-        <v>1</v>
-      </c>
-      <c r="F98">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="99" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>15541</v>
       </c>
       <c r="B99" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C99" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D99">
         <v>6</v>
       </c>
       <c r="E99">
-        <v>1</v>
-      </c>
-      <c r="F99">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="100" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>115761</v>
       </c>
       <c r="B100" t="s">
+        <v>143</v>
+      </c>
+      <c r="C100" t="s">
         <v>144</v>
-      </c>
-      <c r="C100" t="s">
-        <v>145</v>
       </c>
       <c r="D100">
         <v>4</v>
@@ -2903,39 +2607,33 @@
       <c r="E100">
         <v>1</v>
       </c>
-      <c r="F100">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="101" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>74212</v>
       </c>
       <c r="B101" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C101" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D101">
         <v>2</v>
       </c>
       <c r="E101">
-        <v>1</v>
-      </c>
-      <c r="F101">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>109780</v>
       </c>
       <c r="B102" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C102" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="D102">
         <v>2</v>
@@ -2943,19 +2641,16 @@
       <c r="E102">
         <v>1</v>
       </c>
-      <c r="F102">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="103" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="103" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>120506</v>
       </c>
       <c r="B103" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C103" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="D103">
         <v>1</v>
@@ -2963,19 +2658,16 @@
       <c r="E103">
         <v>1</v>
       </c>
-      <c r="F103">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="104" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>36036</v>
       </c>
       <c r="B104" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C104" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="D104">
         <v>5</v>
@@ -2983,19 +2675,16 @@
       <c r="E104">
         <v>1</v>
       </c>
-      <c r="F104">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="105" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="105" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>64978</v>
       </c>
       <c r="B105" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C105" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D105">
         <v>10</v>
@@ -3003,19 +2692,16 @@
       <c r="E105">
         <v>1</v>
       </c>
-      <c r="F105">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="106" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
         <v>112142</v>
       </c>
       <c r="B106" t="s">
+        <v>150</v>
+      </c>
+      <c r="C106" t="s">
         <v>151</v>
-      </c>
-      <c r="C106" t="s">
-        <v>152</v>
       </c>
       <c r="D106">
         <v>4</v>
@@ -3023,19 +2709,16 @@
       <c r="E106">
         <v>1</v>
       </c>
-      <c r="F106">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="107" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
         <v>73892</v>
       </c>
       <c r="B107" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C107" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D107">
         <v>5</v>
@@ -3043,59 +2726,50 @@
       <c r="E107">
         <v>1</v>
       </c>
-      <c r="F107">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="108" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>137606</v>
       </c>
       <c r="B108" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C108" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="D108">
         <v>0</v>
       </c>
       <c r="E108">
-        <v>1</v>
-      </c>
-      <c r="F108">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>47751</v>
       </c>
       <c r="B109" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C109" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="D109">
         <v>19</v>
       </c>
       <c r="E109">
-        <v>1</v>
-      </c>
-      <c r="F109">
         <v>-1</v>
       </c>
     </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>136587</v>
       </c>
       <c r="B110" t="s">
+        <v>155</v>
+      </c>
+      <c r="C110" t="s">
         <v>156</v>
-      </c>
-      <c r="C110" t="s">
-        <v>157</v>
       </c>
       <c r="D110">
         <v>4</v>
@@ -3103,19 +2777,16 @@
       <c r="E110">
         <v>1</v>
       </c>
-      <c r="F110">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="111" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>127827</v>
       </c>
       <c r="B111" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C111" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D111">
         <v>1</v>
@@ -3123,19 +2794,16 @@
       <c r="E111">
         <v>1</v>
       </c>
-      <c r="F111">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="112" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>75441</v>
       </c>
       <c r="B112" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="C112" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="D112">
         <v>12</v>
@@ -3143,59 +2811,50 @@
       <c r="E112">
         <v>1</v>
       </c>
-      <c r="F112">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="113" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>52382</v>
       </c>
       <c r="B113" t="s">
+        <v>159</v>
+      </c>
+      <c r="C113" t="s">
         <v>160</v>
-      </c>
-      <c r="C113" t="s">
-        <v>161</v>
       </c>
       <c r="D113">
         <v>2</v>
       </c>
       <c r="E113">
-        <v>1</v>
-      </c>
-      <c r="F113">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <v>47100</v>
       </c>
       <c r="B114" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C114" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D114">
         <v>1</v>
       </c>
       <c r="E114">
-        <v>1</v>
-      </c>
-      <c r="F114">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
         <v>131732</v>
       </c>
       <c r="B115" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="C115" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D115">
         <v>3</v>
@@ -3203,64 +2862,58 @@
       <c r="E115">
         <v>1</v>
       </c>
-      <c r="F115">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+    </row>
+    <row r="116" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
         <v>97058</v>
       </c>
       <c r="B116" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="C116" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D116">
         <v>5</v>
       </c>
       <c r="E116">
-        <v>1</v>
-      </c>
-      <c r="F116">
         <v>-1</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A117" s="1"/>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A118" s="1"/>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A119" s="1"/>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A120" s="1"/>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A121" s="1"/>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A122" s="1"/>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A123" s="1"/>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A124" s="1"/>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A125" s="1"/>
     </row>
-    <row r="126" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A126" s="1"/>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A127" s="1"/>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A128" s="1"/>
     </row>
     <row r="129" spans="1:1" x14ac:dyDescent="0.2">
@@ -4384,5 +4037,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
merged in new annotations, cleaned up code
</commit_message>
<xml_diff>
--- a/data/fptp_labeled.xlsx
+++ b/data/fptp_labeled.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10910"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11111"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/elliotsilva/Desktop/DS-GA-1006/FairFrame/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/echo/Documents/2019-20/NYU/Fall/Capstone/FairFrame/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7B3C93BA-0C13-BF4C-A0F2-2C662CB266D8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{993A2012-9659-CD4F-81A6-18597BF665D2}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="680" yWindow="460" windowWidth="28800" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16060" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -901,8 +901,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E501"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="134" zoomScaleNormal="200" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="A103" zoomScale="134" zoomScaleNormal="200" workbookViewId="0">
+      <selection activeCell="E116" sqref="E116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -990,7 +990,7 @@
         <v>7</v>
       </c>
       <c r="E5">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
@@ -1007,7 +1007,7 @@
         <v>6</v>
       </c>
       <c r="E6">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
@@ -1058,7 +1058,7 @@
         <v>0</v>
       </c>
       <c r="E9">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
@@ -1075,7 +1075,7 @@
         <v>5</v>
       </c>
       <c r="E10">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -1092,7 +1092,7 @@
         <v>1</v>
       </c>
       <c r="E11">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -1109,7 +1109,7 @@
         <v>3</v>
       </c>
       <c r="E12">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -1126,7 +1126,7 @@
         <v>0</v>
       </c>
       <c r="E13">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -1160,7 +1160,7 @@
         <v>5</v>
       </c>
       <c r="E15">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
@@ -1296,7 +1296,7 @@
         <v>17</v>
       </c>
       <c r="E23">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.2">
@@ -1313,7 +1313,7 @@
         <v>0</v>
       </c>
       <c r="E24">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
@@ -1381,7 +1381,7 @@
         <v>3</v>
       </c>
       <c r="E28">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.2">
@@ -1398,7 +1398,7 @@
         <v>0</v>
       </c>
       <c r="E29">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.2">
@@ -1466,7 +1466,7 @@
         <v>0</v>
       </c>
       <c r="E33">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.2">
@@ -1483,7 +1483,7 @@
         <v>0</v>
       </c>
       <c r="E34">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -1517,7 +1517,7 @@
         <v>0</v>
       </c>
       <c r="E36">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.2">
@@ -1534,7 +1534,7 @@
         <v>4</v>
       </c>
       <c r="E37">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.2">
@@ -1551,7 +1551,7 @@
         <v>0</v>
       </c>
       <c r="E38">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.2">
@@ -1585,7 +1585,7 @@
         <v>2</v>
       </c>
       <c r="E40">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -1602,7 +1602,7 @@
         <v>7</v>
       </c>
       <c r="E41">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -1619,7 +1619,7 @@
         <v>20</v>
       </c>
       <c r="E42">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -1670,7 +1670,7 @@
         <v>0</v>
       </c>
       <c r="E45">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -1721,7 +1721,7 @@
         <v>2</v>
       </c>
       <c r="E48">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
@@ -1755,7 +1755,7 @@
         <v>19</v>
       </c>
       <c r="E50">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
@@ -1772,7 +1772,7 @@
         <v>3</v>
       </c>
       <c r="E51">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -1840,7 +1840,7 @@
         <v>0</v>
       </c>
       <c r="E55">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
@@ -1891,7 +1891,7 @@
         <v>1</v>
       </c>
       <c r="E58">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
@@ -1942,7 +1942,7 @@
         <v>11</v>
       </c>
       <c r="E61">
-        <v>-1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
@@ -2027,7 +2027,7 @@
         <v>0</v>
       </c>
       <c r="E66">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:5" x14ac:dyDescent="0.2">
@@ -2231,7 +2231,7 @@
         <v>5</v>
       </c>
       <c r="E78">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="79" spans="1:5" x14ac:dyDescent="0.2">
@@ -2333,7 +2333,7 @@
         <v>6</v>
       </c>
       <c r="E84">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="85" spans="1:5" x14ac:dyDescent="0.2">
@@ -2452,7 +2452,7 @@
         <v>4</v>
       </c>
       <c r="E91">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="92" spans="1:5" x14ac:dyDescent="0.2">
@@ -2758,7 +2758,7 @@
         <v>19</v>
       </c>
       <c r="E109">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
@@ -2877,7 +2877,7 @@
         <v>5</v>
       </c>
       <c r="E116">
-        <v>-1</v>
+        <v>1</v>
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">

</xml_diff>